<commit_message>
Message Receipt with No errors
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/alaska/AlaskaCriminalCaseMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl/alaska/AlaskaCriminalCaseMapping.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tizzl\git\main\shared\ojb-resources-common\src\main\resources\ssp\Prosecution_Decision_Reporting\artifacts\service_model\information_model\IEPD\documentation\impl\alaska\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5460" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="-28800" yWindow="5460" windowWidth="24240" windowHeight="13740" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Codes Sets" sheetId="3" r:id="rId1"/>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId2"/>
-    <sheet name="Court Case Filing Update" sheetId="2" r:id="rId3"/>
-    <sheet name="DocumentType" sheetId="4" r:id="rId4"/>
-    <sheet name="DocumentActionType" sheetId="5" r:id="rId5"/>
-    <sheet name="IdentificationCategoryText" sheetId="7" r:id="rId6"/>
-    <sheet name="ChargeApplicabilityText" sheetId="8" r:id="rId7"/>
-    <sheet name="Karpel Mapping" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId3"/>
+    <sheet name="Court Case Filing Update" sheetId="2" r:id="rId4"/>
+    <sheet name="DocumentType" sheetId="4" r:id="rId5"/>
+    <sheet name="DocumentActionType" sheetId="5" r:id="rId6"/>
+    <sheet name="IdentificationCategoryText" sheetId="7" r:id="rId7"/>
+    <sheet name="ChargeApplicabilityText" sheetId="8" r:id="rId8"/>
+    <sheet name="Karpel Mapping" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Court Case Filing'!$B$1:$B$111</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Karpel Mapping'!$A$2:$AE$198</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Karpel Mapping'!$A$2:$AE$198</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2117,7 +2123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -2980,6 +2986,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3027,7 +3036,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3062,7 +3071,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3317,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E107" sqref="E107:E123"/>
     </sheetView>
   </sheetViews>
@@ -5221,9 +5230,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5901,7 +5922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -5969,11 +5990,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -6017,7 +6038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -6074,7 +6095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -6112,7 +6133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE198"/>
   <sheetViews>
@@ -9315,7 +9336,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="91" spans="2:31" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:31" ht="33.75" x14ac:dyDescent="0.2">
       <c r="E91" s="25" t="s">
         <v>374</v>
       </c>
@@ -11951,7 +11972,7 @@
       </c>
       <c r="AE165" s="35"/>
     </row>
-    <row r="166" spans="1:31" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:31" ht="33.75" x14ac:dyDescent="0.2">
       <c r="E166" s="25" t="s">
         <v>374</v>
       </c>

</xml_diff>